<commit_message>
Broschüretext fertig, Projekt läuft
</commit_message>
<xml_diff>
--- a/Dokumentation/ByteOrderSensordaten.xlsx
+++ b/Dokumentation/ByteOrderSensordaten.xlsx
@@ -390,7 +390,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="A1:D2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -417,16 +417,16 @@
     </row>
     <row r="2" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="C2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>